<commit_message>
import job interview excel
</commit_message>
<xml_diff>
--- a/public/sample_excel/job-and-interview.xlsx
+++ b/public/sample_excel/job-and-interview.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Al-hiraa\public\sample_excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F6CC67-3F57-4493-A274-7B6F39704F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="3315" yWindow="3795" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>job_name</t>
   </si>
@@ -25,9 +31,6 @@
   </si>
   <si>
     <t>contract</t>
-  </si>
-  <si>
-    <t>benefits</t>
   </si>
   <si>
     <t>salary</t>
@@ -58,12 +61,6 @@
     <t>SAUDI ARABIA</t>
   </si>
   <si>
-    <t>vendor_first_name</t>
-  </si>
-  <si>
-    <t>vendor_last_name</t>
-  </si>
-  <si>
     <t>vendor_email</t>
   </si>
   <si>
@@ -73,12 +70,6 @@
     <t>JUICE MAKER</t>
   </si>
   <si>
-    <t>New</t>
-  </si>
-  <si>
-    <t>Vendor</t>
-  </si>
-  <si>
     <t>vendor@yopmai.com</t>
   </si>
   <si>
@@ -92,13 +83,16 @@
   </si>
   <si>
     <t>22-08-2024</t>
+  </si>
+  <si>
+    <t>benifits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +119,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -143,10 +145,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -157,8 +160,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -175,9 +180,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,7 +220,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -287,7 +292,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -460,11 +465,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,15 +483,13 @@
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,45 +500,39 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="180" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -544,7 +541,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>1500</v>
@@ -553,41 +550,38 @@
         <v>7000</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{3FFFBB93-07CC-4D88-B1A2-528243599E8F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -599,7 +593,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Add 'Mobile' option to source seeder, fix route casing, and enhance candidate data handling
</commit_message>
<xml_diff>
--- a/public/sample_excel/job-and-interview.xlsx
+++ b/public/sample_excel/job-and-interview.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Al-hiraa\public\sample_excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F6CC67-3F57-4493-A274-7B6F39704F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="3795" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3315" yWindow="3795" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +36,6 @@
     <t>job_description</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>quantity_of_people_required</t>
   </si>
   <si>
@@ -79,19 +70,22 @@
     <t>interview_end_date</t>
   </si>
   <si>
-    <t>14-08-2024</t>
-  </si>
-  <si>
-    <t>22-08-2024</t>
-  </si>
-  <si>
     <t>benifits</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>14-12-2024</t>
+  </si>
+  <si>
+    <t>22-12-2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,9 +174,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -220,7 +214,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -292,7 +286,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -465,11 +459,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +494,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -512,27 +506,27 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
       <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
       <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -541,7 +535,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>1500</v>
@@ -550,30 +544,30 @@
         <v>7000</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{3FFFBB93-07CC-4D88-B1A2-528243599E8F}"/>
+    <hyperlink ref="J2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -581,7 +575,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -593,7 +587,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
benfits change to numeriv
</commit_message>
<xml_diff>
--- a/public/sample_excel/job-and-interview.xlsx
+++ b/public/sample_excel/job-and-interview.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>job_name</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>quantity_of_people_required</t>
-  </si>
-  <si>
-    <t>Wordpress Developer</t>
-  </si>
-  <si>
-    <t>ACCOMODATION +TRANSPORTATION</t>
   </si>
   <si>
     <t>CANDIDATES SHOULD HAVE KNOWLEDGE ABOUT CUTTING,CHOPPING,KITCHEN CLEANING AND ORGANISING.
@@ -76,17 +70,29 @@
     <t>location</t>
   </si>
   <si>
-    <t>14-12-2024</t>
-  </si>
-  <si>
-    <t>22-12-2024</t>
+    <t>interview_location</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>31-01-2025</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>Laravel Developer</t>
+  </si>
+  <si>
+    <t>26-01-2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +127,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -143,7 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -155,6 +167,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -460,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,15 +490,16 @@
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +510,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -505,28 +521,31 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>18</v>
+      <c r="H1" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
       <c r="K1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -535,7 +554,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <v>1500</v>
@@ -544,30 +563,33 @@
         <v>7000</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2">
         <v>5</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="K2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
         <v>19</v>
-      </c>
-      <c r="M2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
feat: Add associate charge to jobs, implement company management, and introduce job/interview data import functionality.
</commit_message>
<xml_diff>
--- a/public/sample_excel/job-and-interview.xlsx
+++ b/public/sample_excel/job-and-interview.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Al-hiraa\public\sample_excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="3315" yWindow="3795" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>job_name</t>
   </si>
@@ -61,9 +66,6 @@
     <t>interview_start_date</t>
   </si>
   <si>
-    <t>interview_end_date</t>
-  </si>
-  <si>
     <t>benifits</t>
   </si>
   <si>
@@ -76,9 +78,6 @@
     <t>Kolkata</t>
   </si>
   <si>
-    <t>31-01-2025</t>
-  </si>
-  <si>
     <t>500</t>
   </si>
   <si>
@@ -86,13 +85,16 @@
   </si>
   <si>
     <t>26-01-2025</t>
+  </si>
+  <si>
+    <t>associate_charge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,13 +113,6 @@
       <color rgb="FF1D1A20"/>
       <name val="Courier New"/>
       <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -153,9 +148,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -165,9 +160,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -231,7 +225,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -266,7 +260,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,15 +482,15 @@
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -510,42 +504,42 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="I1" s="6" t="s">
         <v>16</v>
       </c>
       <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -554,42 +548,42 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>1500</v>
       </c>
       <c r="F2">
+        <v>1500</v>
+      </c>
+      <c r="G2">
         <v>7000</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>5</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
       <c r="N2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="L2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>